<commit_message>
Second experiment added, introduction changed, small fixes
Full code and pdf generated.
</commit_message>
<xml_diff>
--- a/sprawozdanie2/Wyniki.xlsx
+++ b/sprawozdanie2/Wyniki.xlsx
@@ -9,21 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="2" r:id="rId1"/>
     <sheet name="1.2" sheetId="4" r:id="rId2"/>
-    <sheet name="3" sheetId="6" r:id="rId3"/>
+    <sheet name="2" sheetId="8" r:id="rId3"/>
+    <sheet name="3" sheetId="6" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Adult_BadStamina" localSheetId="2">'3'!$A$16:$O$29</definedName>
-    <definedName name="Adult_BadStamina_AND_BadStrength" localSheetId="2">'3'!$A$31:$O$44</definedName>
-    <definedName name="Adult_BadStamina_OR_BadStrength" localSheetId="2">'3'!$A$46:$O$59</definedName>
-    <definedName name="Adult_BadStrenght" localSheetId="2">'3'!$A$1:$O$14</definedName>
+    <definedName name="Adult_BadStamina" localSheetId="3">'3'!$A$16:$O$29</definedName>
+    <definedName name="Adult_BadStamina_AND_BadStrength" localSheetId="3">'3'!$A$31:$O$44</definedName>
+    <definedName name="Adult_BadStamina_OR_BadStrength" localSheetId="3">'3'!$A$46:$O$59</definedName>
+    <definedName name="Adult_BadStrenght" localSheetId="3">'3'!$A$1:$O$14</definedName>
+    <definedName name="AgeAdult_FKAccuDecents" localSheetId="2">'2'!$A$1:$O$14</definedName>
+    <definedName name="Every_FKAccuDecents" localSheetId="2">'2'!$A$16:$O$29</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -120,11 +123,53 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="5" name="AgeAdult_FKAccuDecents" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\2\AgeAdult_FKAccuDecents.csv" decimal="," thousands=" " semicolon="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="Every_FKAccuDecents" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\2\Every_FKAccuDecents.csv" decimal="," thousands=" " semicolon="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="152">
   <si>
     <t>Age: Adult -&gt; Strength: Bad Strength</t>
   </si>
@@ -497,6 +542,90 @@
   <si>
     <t>aa</t>
   </si>
+  <si>
+    <t>Age: Adult -&gt; Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Less than 1000 of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around one third of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 40% of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 1500 of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 3000 of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>More than 5000 of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 20% of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Majority of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>No of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>All of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around half of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around three quaters of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Less than a third of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Every: Every -&gt; Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Less than 1000 are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around one third are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Less than a third are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 1500 are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 3000 are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>More than 5000 are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 20% are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around 40% are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Majority are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>No are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>All are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around half are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
+  <si>
+    <t>Around three quaters are/have Fk Accuracy: Decent Free Kick</t>
+  </si>
 </sst>
 </file>
 
@@ -545,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -553,6 +682,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1977,6 +2107,1188 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:rPr>
+              <a:t>Around 1/3 soccer players have Decent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" baseline="0">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:rPr>
+              <a:t> Free Kick</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL" sz="1400">
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Adult</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2'!$D$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>T2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>T3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>T4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>T5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>T6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>T7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2'!$D$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.58670108893518502</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52683841782975704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.483562152133581</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.483562152133581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99881392398080204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F920-4C58-8F08-930B3520454B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Brak kwalifikatora</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2'!$D$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>T2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>T3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>T4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>T5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>T6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>T7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2'!$D$18:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.94803890276802305</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52683841782975704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47316158217024301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47316158217024301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99881392398080204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F920-4C58-8F08-930B3520454B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="644624384"/>
+        <c:axId val="612735744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="644624384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Miara podsumowania</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="900">
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="612735744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="612735744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:tint val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="644624384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:rPr>
+              <a:t>X soccer players </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>have Decent Free Kick</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL" sz="1400">
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Around 1500 - Adult</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2'!$D$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>T2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>T3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>T4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>T5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>T6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>T7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2'!$D$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52683841782975704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.483562152133581</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.483562152133581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98896673470513596</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99448336735256804</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99881392398080204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D35C-4FBD-A2E3-AAC239AFEBF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Less than 1000 - brak kwalifikatora</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2'!$D$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>T2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>T3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>T4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>T5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>T6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>T7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2'!$D$17:$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52683841782975704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47316158217024301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47316158217024301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94483367352568004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69686103602361105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99881392398080204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D35C-4FBD-A2E3-AAC239AFEBF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="644874752"/>
+        <c:axId val="644760128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="644874752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Miara podsumowania</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="900">
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="644760128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="644760128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:tint val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="644874752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
@@ -2849,7 +4161,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
@@ -3874,6 +5186,80 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4881,6 +6267,886 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="102">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:lineWidthScale>3</cs:lineWidthScale>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="95000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="5000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="102">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:lineWidthScale>3</cs:lineWidthScale>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="95000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="5000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5431,7 +7697,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6059,6 +8325,75 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6115050</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>990599</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>791308</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>162010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>448235</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
@@ -6140,7 +8475,138 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="C1" t="str">
+            <v>T1</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>T2</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>T3</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>T4</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>T5</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>T6</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>T7</v>
+          </cell>
+          <cell r="J1" t="str">
+            <v>T8</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6">
+            <v>0.58399999999999996</v>
+          </cell>
+          <cell r="D6">
+            <v>0.19400000000000001</v>
+          </cell>
+          <cell r="E6">
+            <v>0.77600000000000002</v>
+          </cell>
+          <cell r="F6">
+            <v>0.16300000000000001</v>
+          </cell>
+          <cell r="G6">
+            <v>1</v>
+          </cell>
+          <cell r="H6">
+            <v>0.8</v>
+          </cell>
+          <cell r="I6">
+            <v>0.9</v>
+          </cell>
+          <cell r="J6">
+            <v>0.999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>8.5000000000000006E-2</v>
+          </cell>
+          <cell r="D11">
+            <v>0.19400000000000001</v>
+          </cell>
+          <cell r="E11">
+            <v>0.77600000000000002</v>
+          </cell>
+          <cell r="F11">
+            <v>0.16300000000000001</v>
+          </cell>
+          <cell r="G11">
+            <v>1</v>
+          </cell>
+          <cell r="H11">
+            <v>0.98699999999999999</v>
+          </cell>
+          <cell r="I11">
+            <v>0.99399999999999999</v>
+          </cell>
+          <cell r="J11">
+            <v>0.999</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20">
+            <v>0.53700000000000003</v>
+          </cell>
+          <cell r="D20">
+            <v>0.19400000000000001</v>
+          </cell>
+          <cell r="E20">
+            <v>0.80600000000000005</v>
+          </cell>
+          <cell r="F20">
+            <v>0.192</v>
+          </cell>
+          <cell r="G20">
+            <v>1</v>
+          </cell>
+          <cell r="H20">
+            <v>0.8</v>
+          </cell>
+          <cell r="I20">
+            <v>0.9</v>
+          </cell>
+          <cell r="J20">
+            <v>0.999</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>1</v>
+          </cell>
+          <cell r="D27">
+            <v>0.19400000000000001</v>
+          </cell>
+          <cell r="E27">
+            <v>0.80600000000000005</v>
+          </cell>
+          <cell r="F27">
+            <v>0.192</v>
+          </cell>
+          <cell r="G27">
+            <v>1</v>
+          </cell>
+          <cell r="H27">
+            <v>6.2E-2</v>
+          </cell>
+          <cell r="I27">
+            <v>6.3E-2</v>
+          </cell>
+          <cell r="J27">
+            <v>0.999</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="1">
@@ -6325,18 +8791,26 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Every_FKAccuDecents" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="AgeAdult_FKAccuDecents" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStamina-OR-BadStrength" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStamina-AND-BadStrength" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStamina" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStrenght" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -6605,7 +9079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -7543,8 +10017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:E31"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7608,40 +10082,40 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>0.56551981343037505</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>0.47106022557053301</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
         <v>0.84</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>0.92</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7652,40 +10126,40 @@
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0.23757765553100199</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
         <v>0.88</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="3">
         <v>0.94</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7696,40 +10170,40 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>0.235777655531002</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
         <v>0.84</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <v>0.92</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7740,40 +10214,40 @@
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>0.23757765553100199</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
         <v>0.88</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <v>0.94</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7784,40 +10258,40 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>0.92227765553100105</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
         <v>0.64</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <v>0.67</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7828,40 +10302,40 @@
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>0.233977655531002</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
         <v>0.8</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>0.9</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7872,40 +10346,40 @@
       <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>0.233977655531002</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
         <v>0.8</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>0.9</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7916,40 +10390,40 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>0.236227655531002</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
         <v>0.85</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>0.92500000000000004</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7960,40 +10434,40 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>0.234727655531002</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>0</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
         <v>0.85</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>0.875</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="5">
         <v>1</v>
       </c>
     </row>
@@ -8004,40 +10478,40 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>0.93222849681747999</v>
       </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
         <v>0.94483367352568004</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
         <v>0.69686103602361105</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="5">
         <v>1</v>
       </c>
     </row>
@@ -8048,40 +10522,40 @@
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>0.242481158592733</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
         <v>0.98896673470513596</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="3">
         <v>0.99448336735256804</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="5">
         <v>1</v>
       </c>
     </row>
@@ -8092,40 +10566,40 @@
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>0.242481158592733</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1">
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
         <v>0.98896673470513596</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <v>0.99448336735256804</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="5">
         <v>1</v>
       </c>
     </row>
@@ -8136,40 +10610,40 @@
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>0.24133094068574301</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>0</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <v>0.80415954101616405</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
         <v>0.18882602545968899</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
         <v>0.97241683676283996</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="3">
         <v>0.97269266839521196</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="5">
         <v>0.99616594031003503</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="5">
         <v>0.92199481436531106</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="5">
         <v>0.99928283775583404</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="5">
         <v>1</v>
       </c>
     </row>
@@ -8377,10 +10851,1560 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="97.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" customWidth="1"/>
+    <col min="13" max="13" width="4" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>0.92171991327321201</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F2">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G2">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0.94483367352568004</v>
+      </c>
+      <c r="J2">
+        <v>0.69686103602361105</v>
+      </c>
+      <c r="K2">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L2">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M2">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.63595983424136304</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.58670108893518502</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>0.49614805564722803</v>
+      </c>
+      <c r="D4">
+        <v>0.38439854808641899</v>
+      </c>
+      <c r="E4">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F4">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G4">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0.88</v>
+      </c>
+      <c r="J4">
+        <v>0.94</v>
+      </c>
+      <c r="K4">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L4">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M4">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.231972575048465</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.98896673470513596</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.99448336735256804</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>0.231972575048465</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F6">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G6">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.98896673470513596</v>
+      </c>
+      <c r="J6">
+        <v>0.99448336735256804</v>
+      </c>
+      <c r="K6">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L6">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M6">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>0.230822357141475</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F7">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G7">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.97241683676283996</v>
+      </c>
+      <c r="J7">
+        <v>0.97269266839521196</v>
+      </c>
+      <c r="K7">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L7">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M7">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>0.22706907198673401</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F8">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G8">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.88</v>
+      </c>
+      <c r="J8">
+        <v>0.94</v>
+      </c>
+      <c r="K8">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L8">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M8">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>0.22571907198673399</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F9">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G9">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0.85</v>
+      </c>
+      <c r="J9">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K9">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L9">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M9">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0.22526907198673399</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F10">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G10">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0.84</v>
+      </c>
+      <c r="J10">
+        <v>0.92</v>
+      </c>
+      <c r="K10">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L10">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M10">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>0.22421907198673399</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F11">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G11">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0.85</v>
+      </c>
+      <c r="J11">
+        <v>0.875</v>
+      </c>
+      <c r="K11">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L11">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M11">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>0.22346907198673399</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F12">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G12">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0.8</v>
+      </c>
+      <c r="J12">
+        <v>0.9</v>
+      </c>
+      <c r="K12">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L12">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M12">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>0.22346907198673399</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F13">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G13">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0.8</v>
+      </c>
+      <c r="J13">
+        <v>0.9</v>
+      </c>
+      <c r="K13">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L13">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M13">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>0.211769071986734</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F14">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G14">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0.64</v>
+      </c>
+      <c r="J14">
+        <v>0.67</v>
+      </c>
+      <c r="K14">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L14">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M14">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.85341010647101001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.94483367352568004</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.69686103602361105</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.82058649712214704</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.94803890276802305</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>0.44496224110135302</v>
+      </c>
+      <c r="D19">
+        <v>0.43071853702403001</v>
+      </c>
+      <c r="E19">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F19">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G19">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0.64</v>
+      </c>
+      <c r="J19">
+        <v>0.67</v>
+      </c>
+      <c r="K19">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>0.163662768246262</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F20">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G20">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0.98896673470513596</v>
+      </c>
+      <c r="J20">
+        <v>0.99448336735256804</v>
+      </c>
+      <c r="K20">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.163662768246262</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.98896673470513596</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.99448336735256804</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>0.162512550339273</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F22">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G22">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0.97241683676283996</v>
+      </c>
+      <c r="J22">
+        <v>0.97269266839521196</v>
+      </c>
+      <c r="K22">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>0.15875926518453101</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F23">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G23">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0.88</v>
+      </c>
+      <c r="J23">
+        <v>0.94</v>
+      </c>
+      <c r="K23">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>0.15875926518453101</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F24">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G24">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0.88</v>
+      </c>
+      <c r="J24">
+        <v>0.94</v>
+      </c>
+      <c r="K24">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>0.15740926518453099</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F25">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G25">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0.85</v>
+      </c>
+      <c r="J25">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K25">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>0.15695926518453099</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F26">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G26">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0.84</v>
+      </c>
+      <c r="J26">
+        <v>0.92</v>
+      </c>
+      <c r="K26">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>0.15590926518453099</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F27">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G27">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0.85</v>
+      </c>
+      <c r="J27">
+        <v>0.875</v>
+      </c>
+      <c r="K27">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>0.15515926518453099</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F28">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G28">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0.8</v>
+      </c>
+      <c r="J28">
+        <v>0.9</v>
+      </c>
+      <c r="K28">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>0.15515926518453099</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F29">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G29">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0.8</v>
+      </c>
+      <c r="J29">
+        <v>0.9</v>
+      </c>
+      <c r="K29">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" t="s">
+        <v>8</v>
+      </c>
+      <c r="J50" t="s">
+        <v>9</v>
+      </c>
+      <c r="K50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L50" t="s">
+        <v>11</v>
+      </c>
+      <c r="M50" t="s">
+        <v>12</v>
+      </c>
+      <c r="N50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="str">
+        <f>A3</f>
+        <v>Around one third of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f t="shared" ref="B51:N51" si="0">B3</f>
+        <v>Around one third</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="3">
+        <v>0.58670108893518502</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+    </row>
+    <row r="52" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="str">
+        <f>A18</f>
+        <v>Around one third are/have Fk Accuracy: Decent Free Kick</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f t="shared" ref="B52:K52" si="1">B18</f>
+        <v>Around one third</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="3">
+        <v>0.94803890276802305</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H52" s="3">
+        <v>1</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.58670108893518502</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0.94803890276802305</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0.52683841782975704</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0.47316158217024301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0.47316158217024301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="3">
+        <v>1</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="E60" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="E61" s="3">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" t="s">
+        <v>5</v>
+      </c>
+      <c r="G64" t="s">
+        <v>6</v>
+      </c>
+      <c r="H64" t="s">
+        <v>7</v>
+      </c>
+      <c r="I64" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" t="s">
+        <v>9</v>
+      </c>
+      <c r="K64" t="s">
+        <v>10</v>
+      </c>
+      <c r="L64" t="s">
+        <v>11</v>
+      </c>
+      <c r="M64" t="s">
+        <v>12</v>
+      </c>
+      <c r="N64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0.98896673470513596</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.99448336735256804</v>
+      </c>
+      <c r="K65" s="1">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="L65" s="1">
+        <v>0.256633750758537</v>
+      </c>
+      <c r="M65" s="1">
+        <v>0.99955866938820503</v>
+      </c>
+      <c r="N65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0.47316158217024301</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0.94483367352568004</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0.69686103602361105</v>
+      </c>
+      <c r="K66" s="1">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="E68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0.52683841782975704</v>
+      </c>
+      <c r="E69" s="3">
+        <v>0.52683841782975704</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="3">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="E70" s="3">
+        <v>0.47316158217024301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" s="3">
+        <v>0.483562152133581</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0.47316158217024301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="3">
+        <v>1</v>
+      </c>
+      <c r="E72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" s="3">
+        <v>0.98896673470513596</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0.94483367352568004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74" s="3">
+        <v>0.99448336735256804</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0.69686103602361105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>37</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0.99881392398080204</v>
+      </c>
+      <c r="E75" s="3">
+        <v>0.99881392398080204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O113"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98:J108"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70:F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Report 2 done, discussion&conclusions added, small mistakes corrected
</commit_message>
<xml_diff>
--- a/sprawozdanie2/Wyniki.xlsx
+++ b/sprawozdanie2/Wyniki.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DD4D57-C691-46C5-B853-1F7548D84C69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="2" r:id="rId1"/>
@@ -28,7 +29,7 @@
     <definedName name="AgeAdult_FKAccuDecents" localSheetId="2">'2'!$A$1:$O$14</definedName>
     <definedName name="Every_FKAccuDecents" localSheetId="2">'2'!$A$16:$O$29</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,8 +39,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Adult-BadStamina" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Adult-BadStamina" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\3\Adult-BadStamina.csv" decimal="," thousands=" " semicolon="1">
       <textFields count="15">
         <textField/>
@@ -60,7 +61,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="Adult-BadStamina-AND-BadStrength" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="Adult-BadStamina-AND-BadStrength" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\3\Adult-BadStamina-AND-BadStrength.csv" decimal="," thousands=" " semicolon="1">
       <textFields count="15">
         <textField/>
@@ -81,7 +82,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="Adult-BadStamina-OR-BadStrength" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="Adult-BadStamina-OR-BadStrength" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\3\Adult-BadStamina-OR-BadStrength.csv" decimal="," thousands=" " semicolon="1">
       <textFields count="15">
         <textField/>
@@ -102,7 +103,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="Adult-BadStrenght" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="Adult-BadStrenght" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\3\Adult-BadStrenght.csv" decimal="," thousands=" " semicolon="1">
       <textFields count="15">
         <textField/>
@@ -123,7 +124,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="AgeAdult_FKAccuDecents" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="AgeAdult_FKAccuDecents" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\2\AgeAdult_FKAccuDecents.csv" decimal="," thousands=" " semicolon="1">
       <textFields count="15">
         <textField/>
@@ -144,7 +145,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="Every_FKAccuDecents" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="Every_FKAccuDecents" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Bartosz\Dysk Google\Studia\Komputerowe Systemy Rozpoznawania\KSR_repo\sprawozdanie2\numbers\2\Every_FKAccuDecents.csv" decimal="," thousands=" " semicolon="1">
       <textFields count="15">
         <textField/>
@@ -630,10 +631,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -677,12 +678,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -749,7 +750,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1336,7 +1336,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1442,17 +1441,16 @@
             </a:r>
             <a:r>
               <a:rPr lang="pl-PL" b="1"/>
-              <a:t>being Light have</a:t>
+              <a:t>being Short</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pl-PL" b="1" baseline="0"/>
-              <a:t> Good Sprint</a:t>
+              <a:t> have High Wage</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2039,7 +2037,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2154,7 +2151,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2441,7 +2437,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2556,7 +2551,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2633,7 +2627,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2745,7 +2738,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3032,7 +3024,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3147,7 +3138,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3224,7 +3214,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3338,7 +3327,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3883,7 +3871,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4006,7 +3993,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4091,7 +4077,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4199,7 +4184,7 @@
               <a:t>X </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="pl-PL" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="none" normalizeH="0" baseline="0" smtClean="0"/>
+              <a:rPr lang="pl-PL" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="none" normalizeH="0" baseline="0"/>
               <a:t>of soccer players being </a:t>
             </a:r>
             <a:r>
@@ -4209,7 +4194,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4754,7 +4738,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4877,7 +4860,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4962,7 +4944,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8265,7 +8246,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8300,7 +8287,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8337,7 +8330,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8369,7 +8368,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8406,7 +8411,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8438,7 +8449,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8475,138 +8492,7 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>T1</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>T2</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>T3</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>T4</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>T5</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>T6</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>T7</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>T8</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>0.58399999999999996</v>
-          </cell>
-          <cell r="D6">
-            <v>0.19400000000000001</v>
-          </cell>
-          <cell r="E6">
-            <v>0.77600000000000002</v>
-          </cell>
-          <cell r="F6">
-            <v>0.16300000000000001</v>
-          </cell>
-          <cell r="G6">
-            <v>1</v>
-          </cell>
-          <cell r="H6">
-            <v>0.8</v>
-          </cell>
-          <cell r="I6">
-            <v>0.9</v>
-          </cell>
-          <cell r="J6">
-            <v>0.999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>8.5000000000000006E-2</v>
-          </cell>
-          <cell r="D11">
-            <v>0.19400000000000001</v>
-          </cell>
-          <cell r="E11">
-            <v>0.77600000000000002</v>
-          </cell>
-          <cell r="F11">
-            <v>0.16300000000000001</v>
-          </cell>
-          <cell r="G11">
-            <v>1</v>
-          </cell>
-          <cell r="H11">
-            <v>0.98699999999999999</v>
-          </cell>
-          <cell r="I11">
-            <v>0.99399999999999999</v>
-          </cell>
-          <cell r="J11">
-            <v>0.999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>0.53700000000000003</v>
-          </cell>
-          <cell r="D20">
-            <v>0.19400000000000001</v>
-          </cell>
-          <cell r="E20">
-            <v>0.80600000000000005</v>
-          </cell>
-          <cell r="F20">
-            <v>0.192</v>
-          </cell>
-          <cell r="G20">
-            <v>1</v>
-          </cell>
-          <cell r="H20">
-            <v>0.8</v>
-          </cell>
-          <cell r="I20">
-            <v>0.9</v>
-          </cell>
-          <cell r="J20">
-            <v>0.999</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>1</v>
-          </cell>
-          <cell r="D27">
-            <v>0.19400000000000001</v>
-          </cell>
-          <cell r="E27">
-            <v>0.80600000000000005</v>
-          </cell>
-          <cell r="F27">
-            <v>0.192</v>
-          </cell>
-          <cell r="G27">
-            <v>1</v>
-          </cell>
-          <cell r="H27">
-            <v>6.2E-2</v>
-          </cell>
-          <cell r="I27">
-            <v>6.3E-2</v>
-          </cell>
-          <cell r="J27">
-            <v>0.999</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="1">
@@ -8644,146 +8530,6 @@
             <v>T11</v>
           </cell>
         </row>
-        <row r="3">
-          <cell r="C3">
-            <v>1</v>
-          </cell>
-          <cell r="D3">
-            <v>0.90400000000000003</v>
-          </cell>
-          <cell r="E3">
-            <v>0.125</v>
-          </cell>
-          <cell r="F3">
-            <v>3.7999999999999999E-2</v>
-          </cell>
-          <cell r="G3">
-            <v>1</v>
-          </cell>
-          <cell r="H3">
-            <v>0.65</v>
-          </cell>
-          <cell r="I3">
-            <v>0.7</v>
-          </cell>
-          <cell r="J3">
-            <v>0.999</v>
-          </cell>
-          <cell r="K3">
-            <v>0.44500000000000001</v>
-          </cell>
-          <cell r="L3">
-            <v>0.999</v>
-          </cell>
-          <cell r="M3">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>1</v>
-          </cell>
-          <cell r="D17">
-            <v>0.91600000000000004</v>
-          </cell>
-          <cell r="E17">
-            <v>0.108</v>
-          </cell>
-          <cell r="F17">
-            <v>5.8000000000000003E-2</v>
-          </cell>
-          <cell r="G17">
-            <v>1</v>
-          </cell>
-          <cell r="H17">
-            <v>0.65</v>
-          </cell>
-          <cell r="I17">
-            <v>0.7</v>
-          </cell>
-          <cell r="J17">
-            <v>0.999</v>
-          </cell>
-          <cell r="K17">
-            <v>0.44500000000000001</v>
-          </cell>
-          <cell r="L17">
-            <v>0.999</v>
-          </cell>
-          <cell r="M17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>1</v>
-          </cell>
-          <cell r="D31">
-            <v>0.91</v>
-          </cell>
-          <cell r="E31">
-            <v>0</v>
-          </cell>
-          <cell r="F31">
-            <v>4.0000000000000001E-3</v>
-          </cell>
-          <cell r="G31">
-            <v>0.5</v>
-          </cell>
-          <cell r="H31">
-            <v>0.65</v>
-          </cell>
-          <cell r="I31">
-            <v>0.7</v>
-          </cell>
-          <cell r="J31">
-            <v>0.999</v>
-          </cell>
-          <cell r="K31">
-            <v>0.44500000000000001</v>
-          </cell>
-          <cell r="L31">
-            <v>0.999</v>
-          </cell>
-          <cell r="M31">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>1</v>
-          </cell>
-          <cell r="D45">
-            <v>0.91</v>
-          </cell>
-          <cell r="E45">
-            <v>0.23300000000000001</v>
-          </cell>
-          <cell r="F45">
-            <v>0.22900000000000001</v>
-          </cell>
-          <cell r="G45">
-            <v>0.5</v>
-          </cell>
-          <cell r="H45">
-            <v>0.65</v>
-          </cell>
-          <cell r="I45">
-            <v>0.7</v>
-          </cell>
-          <cell r="J45">
-            <v>0.999</v>
-          </cell>
-          <cell r="K45">
-            <v>0.44500000000000001</v>
-          </cell>
-          <cell r="L45">
-            <v>0.999</v>
-          </cell>
-          <cell r="M45">
-            <v>1</v>
-          </cell>
-        </row>
       </sheetData>
     </sheetDataSet>
   </externalBook>
@@ -8791,27 +8537,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Every_FKAccuDecents" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Every_FKAccuDecents" connectionId="6" xr16:uid="{00000000-0016-0000-0200-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="AgeAdult_FKAccuDecents" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="AgeAdult_FKAccuDecents" connectionId="5" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStamina-OR-BadStrength" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Adult-BadStamina-OR-BadStrength" connectionId="3" xr16:uid="{00000000-0016-0000-0300-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStamina-AND-BadStrength" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Adult-BadStamina-AND-BadStrength" connectionId="2" xr16:uid="{00000000-0016-0000-0300-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStamina" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Adult-BadStamina" connectionId="1" xr16:uid="{00000000-0016-0000-0300-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Adult-BadStrenght" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Adult-BadStrenght" connectionId="4" xr16:uid="{00000000-0016-0000-0300-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9076,22 +8822,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="103.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="1" max="1" width="103.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -9135,7 +8881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -9179,7 +8925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -9223,7 +8969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -9267,7 +9013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -9311,7 +9057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -9355,7 +9101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -9399,7 +9145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -9443,7 +9189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -9487,7 +9233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -9531,7 +9277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -9575,7 +9321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -9619,7 +9365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -9663,7 +9409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -9707,7 +9453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
@@ -9721,7 +9467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -9735,7 +9481,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -9749,7 +9495,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -9763,7 +9509,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -9777,7 +9523,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -9791,7 +9537,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -9805,7 +9551,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -9819,7 +9565,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>22</v>
       </c>
@@ -9833,7 +9579,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>26</v>
       </c>
@@ -9847,7 +9593,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>14</v>
       </c>
@@ -9861,7 +9607,7 @@
         <v>0.69686103602361105</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -9875,7 +9621,7 @@
         <v>0.99448336735256804</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>18</v>
       </c>
@@ -9889,7 +9635,7 @@
         <v>0.99448336735256804</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -9903,7 +9649,7 @@
         <v>0.97269266839521196</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="K32" s="5"/>
@@ -9911,7 +9657,7 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="K33" s="5"/>
@@ -9919,7 +9665,7 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="K34" s="5"/>
@@ -9927,7 +9673,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="K35" s="5"/>
@@ -9935,7 +9681,7 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="K36" s="5"/>
@@ -9943,7 +9689,7 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="K37" s="5"/>
@@ -9951,7 +9697,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="K38" s="5"/>
@@ -9959,7 +9705,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="K39" s="5"/>
@@ -9967,7 +9713,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="K40" s="5"/>
@@ -9975,7 +9721,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="K41" s="5"/>
@@ -9983,7 +9729,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="K42" s="5"/>
@@ -9991,7 +9737,7 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="K43" s="5"/>
@@ -9999,7 +9745,7 @@
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="K44" s="5"/>
@@ -10014,24 +9760,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="105.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="1" max="1" width="105.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -10075,7 +9821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -10119,7 +9865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -10163,7 +9909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -10207,7 +9953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -10251,7 +9997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -10295,7 +10041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -10339,7 +10085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -10383,7 +10129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -10427,7 +10173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -10471,7 +10217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -10515,7 +10261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -10559,7 +10305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -10603,7 +10349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -10647,7 +10393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
@@ -10661,7 +10407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -10675,7 +10421,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -10689,7 +10435,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -10703,7 +10449,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -10717,7 +10463,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -10731,7 +10477,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>24</v>
       </c>
@@ -10745,7 +10491,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>25</v>
       </c>
@@ -10759,7 +10505,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -10773,7 +10519,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -10787,7 +10533,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -10801,7 +10547,7 @@
         <v>0.69686103602361105</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>17</v>
       </c>
@@ -10815,7 +10561,7 @@
         <v>0.99448336735256804</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>18</v>
       </c>
@@ -10829,7 +10575,7 @@
         <v>0.99448336735256804</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>19</v>
       </c>
@@ -10850,26 +10596,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="97.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="97.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
     <col min="13" max="13" width="4" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
@@ -10913,7 +10659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -10957,7 +10703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>126</v>
       </c>
@@ -11001,7 +10747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -11045,7 +10791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -11089,7 +10835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -11133,7 +10879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -11177,7 +10923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -11221,7 +10967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -11265,7 +11011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -11309,7 +11055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -11353,7 +11099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -11397,7 +11143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -11441,7 +11187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -11485,7 +11231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -11529,7 +11275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>139</v>
       </c>
@@ -11564,7 +11310,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
@@ -11599,7 +11345,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>141</v>
       </c>
@@ -11634,7 +11380,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -11669,7 +11415,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>143</v>
       </c>
@@ -11704,7 +11450,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -11739,7 +11485,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -11774,7 +11520,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -11809,7 +11555,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -11844,7 +11590,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -11879,7 +11625,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -11914,7 +11660,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -11949,7 +11695,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -11984,7 +11730,7 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>2</v>
       </c>
@@ -12022,13 +11768,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="str">
         <f>A3</f>
         <v>Around one third of soccer players being/having Age: Adult are/have Fk Accuracy: Decent Free Kick</v>
       </c>
       <c r="B51" s="1" t="str">
-        <f t="shared" ref="B51:N51" si="0">B3</f>
+        <f t="shared" ref="B51" si="0">B3</f>
         <v>Around one third</v>
       </c>
       <c r="C51" s="7"/>
@@ -12060,13 +11806,13 @@
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
     </row>
-    <row r="52" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="str">
         <f>A18</f>
         <v>Around one third are/have Fk Accuracy: Decent Free Kick</v>
       </c>
       <c r="B52" s="1" t="str">
-        <f t="shared" ref="B52:K52" si="1">B18</f>
+        <f t="shared" ref="B52" si="1">B18</f>
         <v>Around one third</v>
       </c>
       <c r="C52" s="7"/>
@@ -12098,7 +11844,7 @@
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>30</v>
       </c>
@@ -12109,7 +11855,7 @@
         <v>0.94803890276802305</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
         <v>31</v>
       </c>
@@ -12120,7 +11866,7 @@
         <v>0.52683841782975704</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>32</v>
       </c>
@@ -12131,7 +11877,7 @@
         <v>0.47316158217024301</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>33</v>
       </c>
@@ -12142,7 +11888,7 @@
         <v>0.47316158217024301</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>34</v>
       </c>
@@ -12153,7 +11899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
         <v>35</v>
       </c>
@@ -12164,7 +11910,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>36</v>
       </c>
@@ -12175,7 +11921,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>37</v>
       </c>
@@ -12186,11 +11932,11 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
         <v>2</v>
       </c>
@@ -12228,7 +11974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
@@ -12269,7 +12015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>139</v>
       </c>
@@ -12301,11 +12047,11 @@
         <v>0.99881392398080204</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
         <v>30</v>
       </c>
@@ -12316,7 +12062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>31</v>
       </c>
@@ -12327,7 +12073,7 @@
         <v>0.52683841782975704</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
         <v>32</v>
       </c>
@@ -12338,7 +12084,7 @@
         <v>0.47316158217024301</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
         <v>33</v>
       </c>
@@ -12349,7 +12095,7 @@
         <v>0.47316158217024301</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
         <v>34</v>
       </c>
@@ -12360,7 +12106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
         <v>35</v>
       </c>
@@ -12371,7 +12117,7 @@
         <v>0.94483367352568004</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
         <v>36</v>
       </c>
@@ -12382,7 +12128,7 @@
         <v>0.69686103602361105</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
         <v>37</v>
       </c>
@@ -12400,28 +12146,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O113"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F70" sqref="F70:F80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12465,7 +12211,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -12509,7 +12255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -12556,7 +12302,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -12600,7 +12346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
@@ -12647,7 +12393,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -12691,7 +12437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -12735,7 +12481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -12779,7 +12525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -12823,7 +12569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -12867,7 +12613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -12911,7 +12657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -12955,7 +12701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -12999,7 +12745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -13043,7 +12789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -13087,7 +12833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -13131,7 +12877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>84</v>
       </c>
@@ -13175,7 +12921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -13222,7 +12968,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -13266,7 +13012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -13310,7 +13056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -13357,7 +13103,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -13401,7 +13147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -13445,7 +13191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -13489,7 +13235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -13533,7 +13279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -13577,7 +13323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -13621,7 +13367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -13665,7 +13411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -13709,7 +13455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -13753,7 +13499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>97</v>
       </c>
@@ -13797,7 +13543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -13841,7 +13587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -13888,7 +13634,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -13932,7 +13678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
@@ -13976,7 +13722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>102</v>
       </c>
@@ -14020,7 +13766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -14067,7 +13813,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>104</v>
       </c>
@@ -14111,7 +13857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -14155,7 +13901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -14199,7 +13945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -14243,7 +13989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -14287,7 +14033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -14331,7 +14077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>109</v>
       </c>
@@ -14375,7 +14121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>110</v>
       </c>
@@ -14419,7 +14165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -14463,7 +14209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>112</v>
       </c>
@@ -14510,7 +14256,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -14557,7 +14303,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -14601,7 +14347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -14645,7 +14391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>116</v>
       </c>
@@ -14689,7 +14435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -14733,7 +14479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>118</v>
       </c>
@@ -14777,7 +14523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -14821,7 +14567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -14865,7 +14611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -14909,7 +14655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
@@ -14956,7 +14702,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>84</v>
       </c>
@@ -15000,7 +14746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>97</v>
       </c>
@@ -15044,7 +14790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>110</v>
       </c>
@@ -15088,7 +14834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F70" t="s">
         <v>30</v>
       </c>
@@ -15105,7 +14851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F71" t="s">
         <v>31</v>
       </c>
@@ -15122,7 +14868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F72" t="s">
         <v>32</v>
       </c>
@@ -15139,7 +14885,7 @@
         <v>0.222263450834879</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F73" t="s">
         <v>33</v>
       </c>
@@ -15156,7 +14902,7 @@
         <v>4.9401041577028897E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F74" t="s">
         <v>34</v>
       </c>
@@ -15173,7 +14919,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F75" t="s">
         <v>35</v>
       </c>
@@ -15190,7 +14936,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F76" t="s">
         <v>36</v>
       </c>
@@ -15207,7 +14953,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F77" t="s">
         <v>37</v>
       </c>
@@ -15224,7 +14970,7 @@
         <v>0.99870623496446598</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F78" t="s">
         <v>38</v>
       </c>
@@ -15241,7 +14987,7 @@
         <v>0.256633750758537</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F79" t="s">
         <v>39</v>
       </c>
@@ -15258,7 +15004,7 @@
         <v>0.99955866938820503</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F80" t="s">
         <v>40</v>
       </c>
@@ -15275,7 +15021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>73</v>
       </c>
@@ -15319,7 +15065,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>87</v>
       </c>
@@ -15360,7 +15106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>101</v>
       </c>
@@ -15401,7 +15147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>109</v>
       </c>
@@ -15442,7 +15188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F98" t="s">
         <v>30</v>
       </c>
@@ -15459,7 +15205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F99" t="s">
         <v>31</v>
       </c>
@@ -15476,7 +15222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F100" t="s">
         <v>32</v>
       </c>
@@ -15493,7 +15239,7 @@
         <v>0.222263450834879</v>
       </c>
     </row>
-    <row r="101" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F101" t="s">
         <v>33</v>
       </c>
@@ -15510,7 +15256,7 @@
         <v>4.9401041577028897E-2</v>
       </c>
     </row>
-    <row r="102" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F102" t="s">
         <v>34</v>
       </c>
@@ -15527,7 +15273,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="103" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F103" t="s">
         <v>35</v>
       </c>
@@ -15544,7 +15290,7 @@
         <v>0.94483367352568004</v>
       </c>
     </row>
-    <row r="104" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F104" t="s">
         <v>36</v>
       </c>
@@ -15561,7 +15307,7 @@
         <v>0.69686103602361105</v>
       </c>
     </row>
-    <row r="105" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F105" t="s">
         <v>37</v>
       </c>
@@ -15578,7 +15324,7 @@
         <v>0.99870623496446598</v>
       </c>
     </row>
-    <row r="106" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F106" t="s">
         <v>38</v>
       </c>
@@ -15595,7 +15341,7 @@
         <v>0.256633750758537</v>
       </c>
     </row>
-    <row r="107" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F107" t="s">
         <v>39</v>
       </c>
@@ -15612,7 +15358,7 @@
         <v>0.99955866938820503</v>
       </c>
     </row>
-    <row r="108" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F108" t="s">
         <v>40</v>
       </c>
@@ -15629,16 +15375,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="6:15" x14ac:dyDescent="0.3">
       <c r="O110" s="1"/>
     </row>
-    <row r="111" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="6:15" x14ac:dyDescent="0.3">
       <c r="O111" s="1"/>
     </row>
-    <row r="112" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="6:15" x14ac:dyDescent="0.3">
       <c r="O112" s="1"/>
     </row>
-    <row r="113" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="15:15" x14ac:dyDescent="0.3">
       <c r="O113" s="1"/>
     </row>
   </sheetData>

</xml_diff>